<commit_message>
Aula 01: Update Files
</commit_message>
<xml_diff>
--- a/Material Complementar/tecnicas-amostragem-aula-01-exemplo.xlsx
+++ b/Material Complementar/tecnicas-amostragem-aula-01-exemplo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Le Bomb\kgalois\FMU\2022.2\2022.2-fmu-tecnicas-amostragem\Material Complementar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7E9806-643D-4CEC-B98F-A519A4F53E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA96C93B-B69C-400B-A736-7574F7B05DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5D0660C-533F-4145-9B52-01E46C6E98BE}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,8 +80,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
-      <sz val="11"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -108,14 +115,133 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -129,16 +255,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D19554A-7CF9-44A6-AA5A-610AAB2888A6}" name="Tabela1" displayName="Tabela1" ref="A1:G4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D19554A-7CF9-44A6-AA5A-610AAB2888A6}" name="Tabela1" displayName="Tabela1" ref="A1:G4" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="A1:G4" xr:uid="{4D19554A-7CF9-44A6-AA5A-610AAB2888A6}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B0D14DBB-6297-4C96-B31B-E2DD46B0DE21}" name="Unidade"/>
-    <tableColumn id="2" xr3:uid="{0B584EEC-E301-4AE2-916C-C4FE8D02FAB0}" name="Nome do Chefe"/>
-    <tableColumn id="3" xr3:uid="{3D1C8EE9-7A38-430E-AFA2-501239597FB0}" name="Sexo"/>
-    <tableColumn id="4" xr3:uid="{65030255-9836-4713-A2D5-B09F43544639}" name="Idade"/>
-    <tableColumn id="5" xr3:uid="{AD67BE39-CA7D-4ED0-9A77-C347EFB258A4}" name="Fumante"/>
-    <tableColumn id="6" xr3:uid="{D7858743-E693-49FF-BA23-72D5ACCA21A0}" name="Renda Bruta Familiar"/>
-    <tableColumn id="7" xr3:uid="{2CD6F1DF-FF46-4E87-93FD-BE9096C89D06}" name="Número de Trabalhadores"/>
+    <tableColumn id="1" xr3:uid="{B0D14DBB-6297-4C96-B31B-E2DD46B0DE21}" name="Unidade" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{0B584EEC-E301-4AE2-916C-C4FE8D02FAB0}" name="Nome do Chefe" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3D1C8EE9-7A38-430E-AFA2-501239597FB0}" name="Sexo" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{65030255-9836-4713-A2D5-B09F43544639}" name="Idade" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{AD67BE39-CA7D-4ED0-9A77-C347EFB258A4}" name="Fumante" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{D7858743-E693-49FF-BA23-72D5ACCA21A0}" name="Renda Bruta Familiar" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{2CD6F1DF-FF46-4E87-93FD-BE9096C89D06}" name="Número de Trabalhadores" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -444,112 +570,115 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>20</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>30</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>30</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>40</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>18</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G12" s="1"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="G12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>